<commit_message>
Navigate to cart started... working on filling out address information
</commit_message>
<xml_diff>
--- a/HansenBeauProject2/Accessory Files/Orders.xlsx
+++ b/HansenBeauProject2/Accessory Files/Orders.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8EF6E4-0CA4-43F9-8FAB-5B88809D70E9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7353B197-9E39-4CD8-A79D-A287A8D05FDC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>Product</t>
   </si>
@@ -82,21 +82,41 @@
     <t>Primary Phone</t>
   </si>
   <si>
-    <t>Beau</t>
-  </si>
-  <si>
-    <t>Hansen</t>
-  </si>
-  <si>
     <t>1111 First Street</t>
+  </si>
+  <si>
+    <t>Billing Address</t>
+  </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>Steve</t>
+  </si>
+  <si>
+    <t>Jobs</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Shipping Address</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -124,9 +144,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,7 +435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -505,63 +531,130 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1">
+        <v>76013</v>
+      </c>
+      <c r="F2" s="1">
+        <v>208</v>
+      </c>
+      <c r="G2" s="1">
+        <v>5554970</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="1">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1">
         <v>76013</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F5" s="1">
         <v>208</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G5" s="1">
         <v>5554970</v>
       </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A4:A5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Insert billling address information implemented
</commit_message>
<xml_diff>
--- a/HansenBeauProject2/Accessory Files/Orders.xlsx
+++ b/HansenBeauProject2/Accessory Files/Orders.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7353B197-9E39-4CD8-A79D-A287A8D05FDC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2A40F2-D3A0-4B61-9B54-D457E7A55BC0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,15 +144,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,7 +529,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -550,7 +545,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -576,7 +571,6 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
       <c r="B2" s="1" t="s">
         <v>21</v>
       </c>
@@ -600,7 +594,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -626,7 +620,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
+      <c r="A5" s="2"/>
       <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
@@ -650,10 +644,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A4:A5"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Populate shipping address information implemented... populate payment information implemented
</commit_message>
<xml_diff>
--- a/HansenBeauProject2/Accessory Files/Orders.xlsx
+++ b/HansenBeauProject2/Accessory Files/Orders.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2A40F2-D3A0-4B61-9B54-D457E7A55BC0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07225E1-4C54-40C9-B216-6C8E9FB45885}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>Product</t>
   </si>
@@ -529,7 +529,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -540,8 +540,7 @@
     <col min="4" max="4" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -610,12 +609,6 @@
         <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -633,13 +626,7 @@
       <c r="E5" s="1">
         <v>76013</v>
       </c>
-      <c r="F5" s="1">
-        <v>208</v>
-      </c>
-      <c r="G5" s="1">
-        <v>5554970</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="F5" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Send SMTP Mail Message set up and sends successfully... Wrting to Excel File for ProductNotFound implemented (need to adjust to fix orchestrator readonly problem)... all assets and credentials created in orchestrator and correctly called... Partial work toward implementing Retry++ and invoking, requires more thinking (how do I want to deal with exceptions in general?)...
</commit_message>
<xml_diff>
--- a/HansenBeauProject2/Accessory Files/Orders.xlsx
+++ b/HansenBeauProject2/Accessory Files/Orders.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07225E1-4C54-40C9-B216-6C8E9FB45885}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649635D6-1E7F-45B5-9564-EE31E6600E39}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" r:id="rId1"/>
@@ -430,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -528,7 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Scrapes Cart Page to get unit price, total price, and subtotal. saves to excel sheet... creating of invoice docx file with populated values (still needs work)... some exception handling with login screen and product ordering... writing to excel sheet completely implemented...
</commit_message>
<xml_diff>
--- a/HansenBeauProject2/Accessory Files/Orders.xlsx
+++ b/HansenBeauProject2/Accessory Files/Orders.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649635D6-1E7F-45B5-9564-EE31E6600E39}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC6BCDC-EDC3-47AC-BD30-97A663B17F84}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>Product</t>
   </si>
@@ -101,6 +101,12 @@
   </si>
   <si>
     <t>Shipping Address</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>Total Price</t>
   </si>
 </sst>
 </file>
@@ -428,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -439,7 +445,7 @@
     <col min="1" max="1" width="25" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -452,8 +458,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -462,7 +474,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -470,7 +482,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -478,7 +490,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -486,7 +498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -494,7 +506,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -502,7 +514,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -510,7 +522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Queues implemented... some invoking done, will finish after i deploy to orchestratot... invoice builds correctly... non-fatal error writing to Orders2.xlsx
</commit_message>
<xml_diff>
--- a/HansenBeauProject2/Accessory Files/Orders.xlsx
+++ b/HansenBeauProject2/Accessory Files/Orders.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC6BCDC-EDC3-47AC-BD30-97A663B17F84}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1D4331-9BEE-4011-8AD7-CEB579A4CCFC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Product</t>
   </si>
@@ -82,9 +82,6 @@
     <t>Primary Phone</t>
   </si>
   <si>
-    <t>1111 First Street</t>
-  </si>
-  <si>
     <t>Billing Address</t>
   </si>
   <si>
@@ -107,6 +104,21 @@
   </si>
   <si>
     <t>Total Price</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>Gates</t>
+  </si>
+  <si>
+    <t>Microsoft Street</t>
+  </si>
+  <si>
+    <t>MicroSoft</t>
+  </si>
+  <si>
+    <t>Apple Avenue</t>
   </si>
 </sst>
 </file>
@@ -436,7 +448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -459,10 +471,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -540,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,7 +561,7 @@
     <col min="1" max="1" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="14.109375" bestFit="1" customWidth="1"/>
@@ -557,7 +569,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>12</v>
@@ -578,35 +590,35 @@
         <v>17</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E2" s="1">
         <v>76013</v>
       </c>
       <c r="F2" s="1">
-        <v>208</v>
+        <v>789</v>
       </c>
       <c r="G2" s="1">
-        <v>5554970</v>
+        <v>55511234</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>12</v>
@@ -621,25 +633,25 @@
         <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E5" s="1">
         <v>76013</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>